<commit_message>
adjust code to  new xlsx files+update loading page
</commit_message>
<xml_diff>
--- a/configuration/vehicles_generating.xlsx
+++ b/configuration/vehicles_generating.xlsx
@@ -428,7 +428,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
@@ -436,7 +436,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">

</xml_diff>